<commit_message>
finish schematics for mega board, and fix error in spreadsheet
</commit_message>
<xml_diff>
--- a/Electronics Assembly/Electronics Materials List.xlsx
+++ b/Electronics Assembly/Electronics Materials List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/080a2f6242e3e4fa/Muntean Research/RotaRod Manuscript/Supplements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre Maia Chagas\Documents\GitHub\sussex\mouseduino\Electronics Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{C10C3738-7094-45B1-B023-F9925BAD48AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6FA933F-10F3-4EFC-8328-F304D7DFFFF7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF09469D-9BB1-4D6E-AB25-5C2FAA0ED69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{F834CFAD-3D68-984F-9B64-84A2073CB4F0}"/>
+    <workbookView xWindow="5280" yWindow="795" windowWidth="21600" windowHeight="11385" xr2:uid="{F834CFAD-3D68-984F-9B64-84A2073CB4F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Electronics" sheetId="2" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>https://www.adafruit.com/product/1609?gclid=Cj0KCQiA_bieBhDSARIsADU4zLcjrpxeF4P4isKgfLrtBxQLvsXbniKkpfEIAtMdjugmabYGUZJLKLsaAiQmEALw_wcB</t>
   </si>
   <si>
-    <t>https://www.amazon.com/ELEGOO-ATmega2560-ATMEGA16U2-Projects-Compliant/dp/B01H4ZLZLQ/ref=sr_1_2_sspa?gclid=Cj0KCQiA_bieBhDSARIsADU4zLcS6eXNGWAINGfcoDVgKMnC42_354Z0Xqn9y6T-XLoOnvL-Arnsr9YaAiCtEALw_wcB&amp;hvadid=570507306139&amp;hvdev=c&amp;hvlocphy=9011165&amp;hvnetw=g&amp;hvqmt=e&amp;hvrand=10337382385117367914&amp;hvtargid=kwd-270409539501&amp;hydadcr=18006_13462244&amp;keywords=elegoo%2Bmega%2B2560&amp;qid=1674528182&amp;sr=8-2-spons&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEzRzRWVDNFSFVVUjJaJmVuY3J5cHRlZElkPUExMDIzMTAxMTZNR0hYUkxPUUw4MiZlbmNyeXB0ZWRBZElkPUEwNDA1MjE3Mk5WUUhXTUtGMDVJOCZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU&amp;th=1</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/ELEGOO-Board-ATmega328P-ATMEGA16U2-Compliant/dp/B01EWOE0UU/ref=sr_1_1_sspa?crid=2CJAVA80GVL12&amp;keywords=arduino+uno&amp;qid=1674528229&amp;sprefix=arduino+uno%2Caps%2C127&amp;sr=8-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyN1BEWjdLMVpLTTdEJmVuY3J5cHRlZElkPUEwMzgyMjMzMkk0WDA5TkFCUjRLRCZlbmNyeXB0ZWRBZElkPUEwNDgzODMzMUlIN1I4WVRSM0w1UiZ3aWRnZXROYW1lPXNwX2F0ZiZhY3Rpb249Y2xpY2tSZWRpcmVjdCZkb05vdExvZ0NsaWNrPXRydWU=</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>https://www.homedepot.com/p/Gardner-Bender-20-Amp-Single-Pole-Toggle-Switch-1-Pack-GSW-121/100117400?source=shoppingads&amp;locale=en-US&amp;&amp;mtc=SHOPPING-CM-CML-GGL-D27-027_002_WIRING_DEVIC-NA-NA-NA-SMART-2997116-NA-NA-NA-NBR-NA-NA-NEW-PL3&amp;cm_mmc=SHOPPING-CM-CML-GGL-D27-027_002_WIRING_DEVIC-NA-NA-NA-SMART-2997116-NA-NA-NA-NBR-NA-NA-NEW-PL3-71700000093390730-58700007789602690-92700070740570989&amp;gclid=Cj0KCQiAic6eBhCoARIsANlox87aIf6_QyrNLHHahJ4B2Al4LPxqtHrTT5lfhgW3zwycTaaq0b_LwBQaApsdEALw_wcB&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/GP2Y0A02YK0F-Infrared-Proximity-20-150cm-Distance/dp/B07WQWHNDW</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -431,10 +431,10 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -444,25 +444,25 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -487,7 +487,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -813,23 +813,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3636F976-5071-4EFF-9C23-3488168A64D5}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="92" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E33"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="92" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.375" customWidth="1"/>
     <col min="2" max="2" width="9.875" customWidth="1"/>
-    <col min="3" max="3" width="50.3125" customWidth="1"/>
+    <col min="3" max="3" width="50.375" customWidth="1"/>
     <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="7" max="7" width="64.8125" customWidth="1"/>
+    <col min="7" max="7" width="64.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -843,9 +843,9 @@
       </c>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -854,7 +854,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -873,15 +873,15 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="11">
         <v>5</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="12">
         <v>0.995</v>
@@ -895,13 +895,13 @@
       </c>
       <c r="G4" s="20"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="13">
         <v>5</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="14">
         <v>0.3</v>
@@ -915,7 +915,7 @@
       </c>
       <c r="G5" s="20"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
@@ -933,17 +933,17 @@
         <v>27.99</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="22"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="17">
         <v>1</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="18">
         <v>9.99</v>
@@ -953,19 +953,19 @@
         <v>9.99</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="22"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="13">
         <v>5</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="14">
         <v>10.45</v>
@@ -975,19 +975,19 @@
         <v>52.25</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="17">
         <v>1</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="18">
         <v>20.99</v>
@@ -997,17 +997,17 @@
         <v>20.99</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="17">
         <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="18">
         <v>16.989999999999998</v>
@@ -1017,19 +1017,19 @@
         <v>16.989999999999998</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="22"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="14">
         <v>4.76</v>
@@ -1039,17 +1039,17 @@
         <v>4.76</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="14">
         <v>1.59</v>
@@ -1059,17 +1059,17 @@
         <v>1.59</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="13">
         <v>2</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="14">
         <v>2.5</v>
@@ -1083,13 +1083,13 @@
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="14">
         <v>2.5</v>
@@ -1103,15 +1103,15 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="17">
         <v>1</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="18">
         <v>17.95</v>
@@ -1121,19 +1121,19 @@
         <v>17.95</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G15" s="22"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="26">
         <v>1</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="27">
         <v>12.2</v>
@@ -1143,17 +1143,17 @@
         <v>12.2</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="26">
         <v>1</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="27">
         <v>9.1199999999999992</v>
@@ -1163,17 +1163,17 @@
         <v>9.1199999999999992</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="28"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="13">
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="14">
         <v>6.42</v>
@@ -1183,17 +1183,17 @@
         <v>6.42</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="13">
         <v>1</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="27">
         <v>3.1E-2</v>
@@ -1203,13 +1203,13 @@
         <v>3.1E-2</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="17">
         <v>2</v>
@@ -1229,13 +1229,13 @@
       </c>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="13">
         <v>2</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="13">
         <v>0.65</v>
@@ -1245,17 +1245,17 @@
         <v>1.3</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" s="20"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="13">
         <v>1</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="14">
         <v>2.4300000000000002</v>
@@ -1265,17 +1265,17 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="20"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="13">
         <v>3</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="14">
         <v>0.1</v>
@@ -1285,17 +1285,17 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G23" s="20"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="13">
         <v>15</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="14">
         <v>0.1</v>
@@ -1305,19 +1305,19 @@
         <v>1.5</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="17">
         <v>1</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="18">
         <v>11.95</v>
@@ -1327,17 +1327,17 @@
         <v>11.95</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="22"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="17">
         <v>1</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D26" s="18">
         <v>15.95</v>
@@ -1347,17 +1347,17 @@
         <v>15.95</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="22"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="17">
         <v>1</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="18">
         <v>9.99</v>
@@ -1367,17 +1367,17 @@
         <v>9.99</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G27" s="22"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="17">
         <v>1</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="18">
         <v>2.95</v>
@@ -1387,17 +1387,17 @@
         <v>2.95</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" s="22"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="17">
         <v>9</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="18">
         <v>1.22</v>
@@ -1407,17 +1407,17 @@
         <v>10.98</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G29" s="22"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="17">
         <v>3</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30" s="18">
         <v>1.98</v>
@@ -1427,17 +1427,17 @@
         <v>5.9399999999999995</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G30" s="22"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="17">
         <v>2</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="18">
         <v>1.95</v>
@@ -1447,13 +1447,13 @@
         <v>3.9</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G31" s="22"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="13">
         <v>1</v>
@@ -1473,13 +1473,13 @@
       </c>
       <c r="G32" s="20"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="13">
         <v>1</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D33" s="14">
         <v>3.85</v>
@@ -1489,16 +1489,16 @@
         <v>3.85</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G33" s="20"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1507,13 +1507,13 @@
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="16">
@@ -1523,11 +1523,11 @@
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="17"/>
       <c r="C42" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="16">
@@ -1537,11 +1537,11 @@
       <c r="F42" s="23"/>
       <c r="G42" s="22"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="17"/>
       <c r="C43" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="16">
@@ -1551,11 +1551,11 @@
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="17"/>
       <c r="C44" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="16">
@@ -1565,13 +1565,13 @@
       <c r="F44" s="22"/>
       <c r="G44" s="22"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="17">
         <v>1</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" s="18">
         <v>19.95</v>
@@ -1581,15 +1581,15 @@
         <v>19.95</v>
       </c>
       <c r="F45" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G45" s="22"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="17"/>
       <c r="C46" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="16">
@@ -1599,7 +1599,7 @@
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="17"/>
       <c r="C47" s="15"/>

</xml_diff>